<commit_message>
First launch version 15 april
</commit_message>
<xml_diff>
--- a/app/static/csv/consent.xlsx
+++ b/app/static/csv/consent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ACA403-8E6E-4B3F-B39C-0F964C693AC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E34837D-EAB1-4CA8-97C1-C3375843AA3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
 gedurende de levensloop </t>
   </si>
   <si>
-    <t>Locatie: Sectie Cognitieve Psychologie, Universiteit Leiden</t>
-  </si>
-  <si>
     <t xml:space="preserve">Over dit onderzoek </t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Als u ervoor kiest om te worden betaald voor deelname</t>
   </si>
   <si>
-    <t xml:space="preserve">Arko Ghosh, Sectie Cognitieve Psychologie. agestudy@fsw.leidenuniv.nl   </t>
-  </si>
-  <si>
     <t>li1</t>
   </si>
   <si>
@@ -305,6 +299,12 @@
   </si>
   <si>
     <t>en als we expliciet een vergoeding via e-mail hebben bevestigd,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arko Ghosh, Afdeling Cognitieve Psychologie. agestudy@fsw.leidenuniv.nl   </t>
+  </si>
+  <si>
+    <t>Locatie: Afdeling Cognitieve Psychologie, Universiteit Leiden</t>
   </si>
 </sst>
 </file>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1227,7 +1227,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1238,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1249,7 +1249,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1257,10 +1257,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
@@ -1271,7 +1271,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1279,10 +1279,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1290,10 +1290,10 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1304,7 +1304,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1315,7 +1315,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1326,7 +1326,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="218" x14ac:dyDescent="0.4">
@@ -1334,21 +1334,21 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -1359,161 +1359,161 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
         <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1522,6 +1522,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D896C3867AA3F4EB0C0DE718E7AD517" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80024e68534539ed8e026f0b5c1f9e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c478e2cf-1bd2-4bab-9bac-f508c15c8b21" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dc892a718835b0a8dea2591f8ec0eaf" ns3:_="">
     <xsd:import namespace="c478e2cf-1bd2-4bab-9bac-f508c15c8b21"/>
@@ -1699,22 +1714,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{795265F2-266D-4586-819E-45E6D5B46E6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABEC6EA6-3305-40CD-97CE-314066B754E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D0E8E4A-0AEB-48AA-BCC2-52A9E4FEE6AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1730,21 +1747,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABEC6EA6-3305-40CD-97CE-314066B754E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{795265F2-266D-4586-819E-45E6D5B46E6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>